<commit_message>
added data from Friday
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -13,10 +13,17 @@
   </bookViews>
   <sheets>
     <sheet name="Objective" sheetId="1" r:id="rId1"/>
-    <sheet name="Subjective" sheetId="2" r:id="rId2"/>
-    <sheet name="Demographic" sheetId="3" r:id="rId3"/>
+    <sheet name="Learning" sheetId="4" r:id="rId2"/>
+    <sheet name="Subjective" sheetId="2" r:id="rId3"/>
+    <sheet name="Demographic" sheetId="3" r:id="rId4"/>
+    <sheet name="Basic Analysis" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <pivotCaches>
+    <pivotCache cacheId="17" r:id="rId6"/>
+    <pivotCache cacheId="21" r:id="rId7"/>
+    <pivotCache cacheId="25" r:id="rId8"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="70">
   <si>
     <t>Participant</t>
   </si>
@@ -143,13 +150,106 @@
   </si>
   <si>
     <t>Concept</t>
+  </si>
+  <si>
+    <t>Errors</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Grad Student</t>
+  </si>
+  <si>
+    <t>Graduate Student / Computer Sciences</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Postdoctorial research associate</t>
+  </si>
+  <si>
+    <t>Programming Languages</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Average of made_task_easy</t>
+  </si>
+  <si>
+    <t>Average of happy</t>
+  </si>
+  <si>
+    <t>Average of useful</t>
+  </si>
+  <si>
+    <t>Average of satisfied</t>
+  </si>
+  <si>
+    <t>Average of accurate</t>
+  </si>
+  <si>
+    <t>Average of confident</t>
+  </si>
+  <si>
+    <t>Average of would_use_again</t>
+  </si>
+  <si>
+    <t>Average of fun</t>
+  </si>
+  <si>
+    <t>Average of easy_to_understand</t>
+  </si>
+  <si>
+    <t>Joystick Total</t>
+  </si>
+  <si>
+    <t>Kinesiological Total</t>
+  </si>
+  <si>
+    <t>Kinesiological+ Total</t>
+  </si>
+  <si>
+    <t>Control x Task</t>
+  </si>
+  <si>
+    <t>Average of Score (max time = 5 min)</t>
+  </si>
+  <si>
+    <t>Average of Task Time (seconds)</t>
+  </si>
+  <si>
+    <t>Sum of Errors</t>
+  </si>
+  <si>
+    <t>Average of Learning Time (only record once)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control </t>
+  </si>
+  <si>
+    <t>Average of Ease of Use</t>
+  </si>
+  <si>
+    <t>Average of Usefulness</t>
+  </si>
+  <si>
+    <t>Average of Enjoyment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,16 +274,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor theme="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -191,19 +305,240 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -220,6 +555,1187 @@
 </styleSheet>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chris" refreshedDate="42345.544865625001" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="12">
+  <cacheSource type="worksheet">
+    <worksheetSource name="learning"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Participant" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="12"/>
+    </cacheField>
+    <cacheField name="Control Type" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Kinesiological+"/>
+        <s v="Kinesiological"/>
+        <s v="Joystick"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Learning Time (only record once)" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="173" maxValue="293"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chris" refreshedDate="42345.544866435186" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="24">
+  <cacheSource type="worksheet">
+    <worksheetSource name="obj"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="Participant" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="12"/>
+    </cacheField>
+    <cacheField name="Control Type" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Kinesiological+"/>
+        <s v="Kinesiological"/>
+        <s v="Joystick"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Task Type" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Movement"/>
+        <s v="Rotation"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Task Time (seconds)" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="31" maxValue="177"/>
+    </cacheField>
+    <cacheField name="Errors" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="1"/>
+    </cacheField>
+    <cacheField name="Score (max time = 5 min)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.41000000000000003" maxValue="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chris" refreshedDate="42345.544866898148" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="24">
+  <cacheSource type="worksheet">
+    <worksheetSource name="sub"/>
+  </cacheSource>
+  <cacheFields count="15">
+    <cacheField name="Participant" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="12"/>
+    </cacheField>
+    <cacheField name="Control Type" numFmtId="0">
+      <sharedItems count="3">
+        <s v="Kinesiological+"/>
+        <s v="Kinesiological"/>
+        <s v="Joystick"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Task Type" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Movement"/>
+        <s v="Rotation"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="made_task_easy" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="6"/>
+    </cacheField>
+    <cacheField name="easy_to_understand" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="7"/>
+    </cacheField>
+    <cacheField name="fun" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="7"/>
+    </cacheField>
+    <cacheField name="would_use_again" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="6"/>
+    </cacheField>
+    <cacheField name="confident" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="6"/>
+    </cacheField>
+    <cacheField name="accurate" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="6"/>
+    </cacheField>
+    <cacheField name="satisfied" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="7"/>
+    </cacheField>
+    <cacheField name="useful" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="6"/>
+    </cacheField>
+    <cacheField name="happy" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="7"/>
+    </cacheField>
+    <cacheField name="Ease of Use" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="3.3333333333333335" maxValue="6.333333333333333"/>
+    </cacheField>
+    <cacheField name="Usefulness" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="3.3333333333333335" maxValue="5.666666666666667"/>
+    </cacheField>
+    <cacheField name="Enjoyment" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="3.6666666666666665" maxValue="7"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="12">
+  <r>
+    <n v="1"/>
+    <x v="0"/>
+    <n v="192"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="0"/>
+    <n v="293"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="0"/>
+    <n v="272"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="0"/>
+    <n v="173"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="1"/>
+    <n v="187"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="2"/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="24">
+  <r>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="35"/>
+    <n v="0"/>
+    <n v="0.8833333333333333"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="36"/>
+    <n v="0"/>
+    <n v="0.88"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="31"/>
+    <n v="0"/>
+    <n v="0.89666666666666672"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="38"/>
+    <n v="0"/>
+    <n v="0.87333333333333329"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="31"/>
+    <n v="0"/>
+    <n v="0.89666666666666672"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="80"/>
+    <n v="0"/>
+    <n v="0.73333333333333339"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="52"/>
+    <n v="0"/>
+    <n v="0.82666666666666666"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="65"/>
+    <n v="0"/>
+    <n v="0.78333333333333333"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="31"/>
+    <n v="0"/>
+    <n v="0.89666666666666672"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="177"/>
+    <n v="1"/>
+    <n v="0.41000000000000003"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <n v="1"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="24">
+  <r>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5.333333333333333"/>
+    <n v="5.333333333333333"/>
+    <n v="5.333333333333333"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="3.6666666666666665"/>
+    <n v="4.333333333333333"/>
+    <n v="4.333333333333333"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="7"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="6.333333333333333"/>
+    <n v="5.333333333333333"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="5.333333333333333"/>
+    <n v="5"/>
+    <n v="6.666666666666667"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="4.333333333333333"/>
+    <n v="5.333333333333333"/>
+    <n v="6.333333333333333"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="7"/>
+    <n v="6"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="4.333333333333333"/>
+    <n v="5.666666666666667"/>
+    <n v="6.333333333333333"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4.333333333333333"/>
+    <n v="4.666666666666667"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="4"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="4.333333333333333"/>
+    <n v="5.333333333333333"/>
+    <n v="3.6666666666666665"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5.333333333333333"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3.3333333333333335"/>
+    <n v="3.3333333333333335"/>
+    <n v="4.666666666666667"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="2"/>
+    <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+    <e v="#DIV/0!"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Control x Task">
+  <location ref="A17:D29" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="15">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Average of Ease of Use" fld="12" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of Usefulness" fld="13" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of Enjoyment" fld="14" subtotal="average" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="learning" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Control ">
+  <location ref="A47:B51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Learning Time (only record once)" fld="2" subtotal="average" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium2" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="objective" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Control x Task">
+  <location ref="A32:D44" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Average of Task Time (seconds)" fld="3" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Sum of Errors" fld="4" baseField="2" baseItem="1"/>
+    <dataField name="Average of Score (max time = 5 min)" fld="5" subtotal="average" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium3" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="subjective" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Control x Task">
+  <location ref="A2:J14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="15">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="default">
+      <x v="2"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+    <i i="5">
+      <x v="5"/>
+    </i>
+    <i i="6">
+      <x v="6"/>
+    </i>
+    <i i="7">
+      <x v="7"/>
+    </i>
+    <i i="8">
+      <x v="8"/>
+    </i>
+  </colItems>
+  <dataFields count="9">
+    <dataField name="Average of made_task_easy" fld="3" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of easy_to_understand" fld="4" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of fun" fld="5" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of would_use_again" fld="6" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of confident" fld="7" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of accurate" fld="8" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of satisfied" fld="9" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of useful" fld="10" subtotal="average" baseField="1" baseItem="0"/>
+    <dataField name="Average of happy" fld="11" subtotal="average" baseField="1" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="obj" displayName="obj" ref="A1:F25" totalsRowShown="0">
   <autoFilter ref="A1:F25"/>
@@ -227,9 +1743,9 @@
     <tableColumn id="1" name="Participant"/>
     <tableColumn id="2" name="Control Type"/>
     <tableColumn id="3" name="Task Type"/>
-    <tableColumn id="4" name="Learning Time (only record once)"/>
     <tableColumn id="5" name="Task Time (seconds)"/>
-    <tableColumn id="6" name="Score (max time = 5 min)" dataDxfId="0">
+    <tableColumn id="7" name="Errors"/>
+    <tableColumn id="6" name="Score (max time = 5 min)" dataDxfId="11">
       <calculatedColumnFormula>1-obj[[#This Row],[Task Time (seconds)]]/300</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -238,9 +1754,21 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="sub" displayName="sub" ref="A3:L27" totalsRowShown="0">
-  <autoFilter ref="A3:L27"/>
-  <tableColumns count="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="learning" displayName="learning" ref="A1:C13" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="A1:C13"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Participant" dataDxfId="5"/>
+    <tableColumn id="2" name="Control Type" dataDxfId="4"/>
+    <tableColumn id="4" name="Learning Time (only record once)" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="sub" displayName="sub" ref="A3:O27" totalsRowShown="0">
+  <autoFilter ref="A3:O27"/>
+  <tableColumns count="15">
     <tableColumn id="1" name="Participant"/>
     <tableColumn id="2" name="Control Type"/>
     <tableColumn id="3" name="Task Type"/>
@@ -253,12 +1781,21 @@
     <tableColumn id="10" name="satisfied"/>
     <tableColumn id="11" name="useful"/>
     <tableColumn id="12" name="happy"/>
+    <tableColumn id="13" name="Ease of Use" dataDxfId="2">
+      <calculatedColumnFormula>AVERAGE(E4,H4,I4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" name="Usefulness" dataDxfId="1">
+      <calculatedColumnFormula>AVERAGE(D4,G4,K4)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" name="Enjoyment" dataDxfId="0">
+      <calculatedColumnFormula>AVERAGE(F4,J4,L4)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="demo" displayName="demo" ref="A1:F13" totalsRowShown="0">
   <autoFilter ref="A1:F13"/>
   <tableColumns count="6">
@@ -539,7 +2076,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,6 +2087,7 @@
     <col min="4" max="4" width="33" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -563,10 +2101,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -577,14 +2115,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
+      <c r="D2">
+        <v>35</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
       <c r="F2">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.8833333333333333</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -592,14 +2136,20 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>13</v>
       </c>
+      <c r="D3">
+        <v>36</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
       <c r="F3">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -607,14 +2157,20 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
+      <c r="D4">
+        <v>31</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
       <c r="F4">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.89666666666666672</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -622,14 +2178,20 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
+      <c r="D5">
+        <v>38</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
       <c r="F5">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.87333333333333329</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -637,14 +2199,20 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
+      <c r="D6">
+        <v>31</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
       <c r="F6">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.89666666666666672</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,14 +2220,20 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
+      <c r="D7">
+        <v>80</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
       <c r="F7">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.73333333333333339</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -667,14 +2241,20 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
+      <c r="D8">
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
       <c r="F8">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.82666666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -682,14 +2262,20 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
+      <c r="D9">
+        <v>65</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
       <c r="F9">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.78333333333333333</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,9 +2288,15 @@
       <c r="C10" t="s">
         <v>12</v>
       </c>
+      <c r="D10">
+        <v>31</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
       <c r="F10">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.89666666666666672</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -717,9 +2309,15 @@
       <c r="C11" t="s">
         <v>13</v>
       </c>
+      <c r="D11">
+        <v>177</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
       <c r="F11">
         <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.41000000000000003</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -817,7 +2415,7 @@
         <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -832,7 +2430,7 @@
         <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
         <v>13</v>
@@ -847,7 +2445,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -862,7 +2460,7 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
@@ -877,7 +2475,7 @@
         <v>11</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -892,7 +2490,7 @@
         <v>11</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
@@ -907,7 +2505,7 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -922,7 +2520,7 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
@@ -942,10 +2540,164 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="4">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,9 +2710,12 @@
     <col min="10" max="10" width="15.85546875" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
     <col min="12" max="12" width="13.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
@@ -992,7 +2747,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
@@ -1024,7 +2779,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1061,96 +2816,417 @@
       <c r="L3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>6</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>5</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:O27" si="0">AVERAGE(E4,H4,I4)</f>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N27" si="1">AVERAGE(D4,G4,K4)</f>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O27" si="2">AVERAGE(F4,J4,L4)</f>
+        <v>5.333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="K5">
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="1"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="2"/>
+        <v>4.333333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <v>6</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6">
+        <v>5</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>7</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>6.333333333333333</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="1"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7">
+        <v>7</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="2"/>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>6</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="1"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="2"/>
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>6</v>
+      </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="2"/>
+        <v>6.333333333333333</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="1"/>
+        <v>4.666666666666667</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>6</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="2"/>
+        <v>3.6666666666666665</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1160,8 +3236,47 @@
       <c r="C12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="1"/>
+        <v>5.333333333333333</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1171,8 +3286,47 @@
       <c r="C13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>4.666666666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1182,8 +3336,20 @@
       <c r="C14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -1193,8 +3359,20 @@
       <c r="C15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O15" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>7</v>
       </c>
@@ -1204,8 +3382,20 @@
       <c r="C16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M16" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O16" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7</v>
       </c>
@@ -1215,8 +3405,20 @@
       <c r="C17" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M17" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O17" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8</v>
       </c>
@@ -1226,8 +3428,20 @@
       <c r="C18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8</v>
       </c>
@@ -1237,93 +3451,201 @@
       <c r="C19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M19" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N19" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O19" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M20" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O20" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M21" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O21" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M22" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O22" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M23" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N23" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O23" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M24" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N24" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O24" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M25" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N25" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O25" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C26" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="M26" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N26" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O26" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
+      </c>
+      <c r="M27" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N27" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O27" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
@@ -1335,12 +3657,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1348,7 +3670,7 @@
     <col min="1" max="1" width="14.42578125" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="44.85546875" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
     <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
@@ -1377,25 +3699,100 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
+      </c>
+      <c r="B6">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1439,4 +3836,705 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:J51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9">
+        <v>5</v>
+      </c>
+      <c r="C8" s="9">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9">
+        <v>6</v>
+      </c>
+      <c r="E8" s="9">
+        <v>6</v>
+      </c>
+      <c r="F8" s="9">
+        <v>4</v>
+      </c>
+      <c r="G8" s="9">
+        <v>5</v>
+      </c>
+      <c r="H8" s="9">
+        <v>4</v>
+      </c>
+      <c r="I8" s="9">
+        <v>5</v>
+      </c>
+      <c r="J8" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4</v>
+      </c>
+      <c r="D9" s="9">
+        <v>5</v>
+      </c>
+      <c r="E9" s="9">
+        <v>4</v>
+      </c>
+      <c r="F9" s="9">
+        <v>3</v>
+      </c>
+      <c r="G9" s="9">
+        <v>3</v>
+      </c>
+      <c r="H9" s="9">
+        <v>4</v>
+      </c>
+      <c r="I9" s="9">
+        <v>3</v>
+      </c>
+      <c r="J9" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="9">
+        <v>4</v>
+      </c>
+      <c r="C10" s="9">
+        <v>5</v>
+      </c>
+      <c r="D10" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="E10" s="9">
+        <v>5</v>
+      </c>
+      <c r="F10" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="G10" s="9">
+        <v>4</v>
+      </c>
+      <c r="H10" s="9">
+        <v>4</v>
+      </c>
+      <c r="I10" s="9">
+        <v>4</v>
+      </c>
+      <c r="J10" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9">
+        <v>4.75</v>
+      </c>
+      <c r="C12" s="9">
+        <v>5.75</v>
+      </c>
+      <c r="D12" s="9">
+        <v>6</v>
+      </c>
+      <c r="E12" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="F12" s="9">
+        <v>5.25</v>
+      </c>
+      <c r="G12" s="9">
+        <v>4.25</v>
+      </c>
+      <c r="H12" s="9">
+        <v>5.25</v>
+      </c>
+      <c r="I12" s="9">
+        <v>5.25</v>
+      </c>
+      <c r="J12" s="9">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="C13" s="9">
+        <v>6</v>
+      </c>
+      <c r="D13" s="9">
+        <v>5.75</v>
+      </c>
+      <c r="E13" s="9">
+        <v>5.25</v>
+      </c>
+      <c r="F13" s="9">
+        <v>4</v>
+      </c>
+      <c r="G13" s="9">
+        <v>3.25</v>
+      </c>
+      <c r="H13" s="9">
+        <v>4.25</v>
+      </c>
+      <c r="I13" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="J13" s="9">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="9">
+        <v>4.625</v>
+      </c>
+      <c r="C14" s="9">
+        <v>5.875</v>
+      </c>
+      <c r="D14" s="9">
+        <v>5.875</v>
+      </c>
+      <c r="E14" s="9">
+        <v>5.375</v>
+      </c>
+      <c r="F14" s="9">
+        <v>4.625</v>
+      </c>
+      <c r="G14" s="9">
+        <v>3.75</v>
+      </c>
+      <c r="H14" s="9">
+        <v>4.75</v>
+      </c>
+      <c r="I14" s="9">
+        <v>5.375</v>
+      </c>
+      <c r="J14" s="9">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C19" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D19" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C20" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D20" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C21" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D21" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C23" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D23" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C24" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D24" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C25" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D25" s="9" t="e">
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="9">
+        <v>5.083333333333333</v>
+      </c>
+      <c r="C27" s="9">
+        <v>5.166666666666667</v>
+      </c>
+      <c r="D27" s="9">
+        <v>5.6666666666666661</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="9">
+        <v>4.4166666666666661</v>
+      </c>
+      <c r="C28" s="9">
+        <v>5.083333333333333</v>
+      </c>
+      <c r="D28" s="9">
+        <v>5.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="9">
+        <v>4.75</v>
+      </c>
+      <c r="C29" s="9">
+        <v>5.125</v>
+      </c>
+      <c r="D29" s="9">
+        <v>5.458333333333333</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="9"/>
+      <c r="D34" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="9">
+        <v>31</v>
+      </c>
+      <c r="C38" s="9">
+        <v>0</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0.97416666666666663</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B39" s="9">
+        <v>177</v>
+      </c>
+      <c r="C39" s="9">
+        <v>1</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0.85250000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="9">
+        <v>104</v>
+      </c>
+      <c r="C40" s="9">
+        <v>1</v>
+      </c>
+      <c r="D40" s="9">
+        <v>0.91333333333333333</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="9">
+        <v>37.25</v>
+      </c>
+      <c r="C42" s="9">
+        <v>0</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0.87583333333333335</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="9">
+        <v>54.75</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0</v>
+      </c>
+      <c r="D43" s="9">
+        <v>0.8175</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="9">
+        <v>46</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.84666666666666668</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="9"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B49" s="9">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50" s="9">
+        <v>232.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="9">
+        <v>223.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added all data and JMP tables
</commit_message>
<xml_diff>
--- a/Data/Data.xlsx
+++ b/Data/Data.xlsx
@@ -20,9 +20,9 @@
   </sheets>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="63" r:id="rId6"/>
-    <pivotCache cacheId="67" r:id="rId7"/>
-    <pivotCache cacheId="71" r:id="rId8"/>
+    <pivotCache cacheId="6" r:id="rId6"/>
+    <pivotCache cacheId="10" r:id="rId7"/>
+    <pivotCache cacheId="13" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="78">
   <si>
     <t>Participant</t>
   </si>
@@ -255,6 +255,18 @@
   </si>
   <si>
     <t>Average of Learning Time (seconds)</t>
+  </si>
+  <si>
+    <t>RA/student/CS+HCI</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Computer Science Major</t>
+  </si>
+  <si>
+    <t>graphics phd</t>
   </si>
 </sst>
 </file>
@@ -709,10 +721,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.1666666666666661</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>4.833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.166666666666667</c:v>
@@ -800,10 +812,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.083333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.25</c:v>
@@ -891,10 +903,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.583333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>#N/A</c:v>
+                  <c:v>5.0833333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.3333333333333339</c:v>
@@ -921,11 +933,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="145186328"/>
-        <c:axId val="145186720"/>
+        <c:axId val="141309416"/>
+        <c:axId val="141305888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="145186328"/>
+        <c:axId val="141309416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +980,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145186720"/>
+        <c:crossAx val="141305888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -976,7 +988,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145186720"/>
+        <c:axId val="141305888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1027,7 +1039,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145186328"/>
+        <c:crossAx val="141309416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1292,10 +1304,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.85250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0.74583333333333335</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.89333333333333331</c:v>
@@ -1322,11 +1334,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="141792040"/>
-        <c:axId val="141793608"/>
+        <c:axId val="141305496"/>
+        <c:axId val="141306672"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141792040"/>
+        <c:axId val="141305496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1369,7 +1381,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141793608"/>
+        <c:crossAx val="141306672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1377,7 +1389,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141793608"/>
+        <c:axId val="141306672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1428,7 +1440,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141792040"/>
+        <c:crossAx val="141305496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1662,6 +1674,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1687,11 +1705,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="141814272"/>
-        <c:axId val="141811920"/>
+        <c:axId val="141304712"/>
+        <c:axId val="141307456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141814272"/>
+        <c:axId val="141304712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1734,7 +1752,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141811920"/>
+        <c:crossAx val="141307456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1742,7 +1760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141811920"/>
+        <c:axId val="141307456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1793,7 +1811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141814272"/>
+        <c:crossAx val="141304712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2027,6 +2045,12 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>44.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>76.25</c:v>
+                </c:pt>
                 <c:pt idx="2">
                   <c:v>32</c:v>
                 </c:pt>
@@ -2052,11 +2076,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="141810352"/>
-        <c:axId val="141815056"/>
+        <c:axId val="141304320"/>
+        <c:axId val="141307848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="141810352"/>
+        <c:axId val="141304320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2099,7 +2123,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141815056"/>
+        <c:crossAx val="141307848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2107,7 +2131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="141815056"/>
+        <c:axId val="141307848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,7 +2182,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="141810352"/>
+        <c:crossAx val="141304320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4556,11 +4580,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chris" refreshedDate="42345.762075347222" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="12">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chris" refreshedDate="42346.750082986109" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="24">
   <cacheSource type="worksheet">
-    <worksheetSource name="learning"/>
+    <worksheetSource name="sub"/>
   </cacheSource>
-  <cacheFields count="3">
+  <cacheFields count="15">
     <cacheField name="Participant" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="12"/>
     </cacheField>
@@ -4571,8 +4595,47 @@
         <s v="Joystick"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Learning Time (seconds)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="134" maxValue="293"/>
+    <cacheField name="Task Type" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Movement"/>
+        <s v="Rotation"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="made_task_easy" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="6"/>
+    </cacheField>
+    <cacheField name="easy_to_understand" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="7"/>
+    </cacheField>
+    <cacheField name="fun" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4" maxValue="7"/>
+    </cacheField>
+    <cacheField name="would_use_again" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="6"/>
+    </cacheField>
+    <cacheField name="confident" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="7"/>
+    </cacheField>
+    <cacheField name="accurate" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="2" maxValue="7"/>
+    </cacheField>
+    <cacheField name="satisfied" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="7"/>
+    </cacheField>
+    <cacheField name="useful" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="7"/>
+    </cacheField>
+    <cacheField name="happy" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4" maxValue="7"/>
+    </cacheField>
+    <cacheField name="Ease of Use" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.3333333333333335" maxValue="6.333333333333333"/>
+    </cacheField>
+    <cacheField name="Usefulness" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="2.6666666666666665" maxValue="6.333333333333333"/>
+    </cacheField>
+    <cacheField name="Enjoyment" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="3.6666666666666665" maxValue="7"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -4584,7 +4647,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chris" refreshedDate="42345.762075347222" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="24">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chris" refreshedDate="42346.750083333332" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="24">
   <cacheSource type="worksheet">
     <worksheetSource name="obj"/>
   </cacheSource>
@@ -4606,13 +4669,13 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Task Time (seconds)" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="21" maxValue="177"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="21" maxValue="177"/>
     </cacheField>
     <cacheField name="Errors" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="3"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="3"/>
     </cacheField>
     <cacheField name="Score (max time = 5 min)" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.41000000000000003" maxValue="1"/>
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" minValue="0.41000000000000003" maxValue="0.92999999999999994"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -4624,11 +4687,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chris" refreshedDate="42345.762076273146" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="24">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Chris" refreshedDate="42346.750084143518" createdVersion="5" refreshedVersion="5" minRefreshableVersion="3" recordCount="12">
   <cacheSource type="worksheet">
-    <worksheetSource name="sub"/>
+    <worksheetSource name="learning"/>
   </cacheSource>
-  <cacheFields count="15">
+  <cacheFields count="3">
     <cacheField name="Participant" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="12"/>
     </cacheField>
@@ -4639,47 +4702,8 @@
         <s v="Joystick"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Task Type" numFmtId="0">
-      <sharedItems count="2">
-        <s v="Movement"/>
-        <s v="Rotation"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="made_task_easy" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="6"/>
-    </cacheField>
-    <cacheField name="easy_to_understand" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="7"/>
-    </cacheField>
-    <cacheField name="fun" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="7"/>
-    </cacheField>
-    <cacheField name="would_use_again" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="6"/>
-    </cacheField>
-    <cacheField name="confident" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="7"/>
-    </cacheField>
-    <cacheField name="accurate" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="6"/>
-    </cacheField>
-    <cacheField name="satisfied" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="7"/>
-    </cacheField>
-    <cacheField name="useful" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="6"/>
-    </cacheField>
-    <cacheField name="happy" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="4" maxValue="7"/>
-    </cacheField>
-    <cacheField name="Ease of Use" numFmtId="0">
-      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="3.3333333333333335" maxValue="6.333333333333333"/>
-    </cacheField>
-    <cacheField name="Usefulness" numFmtId="0">
-      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="2.6666666666666665" maxValue="5.666666666666667"/>
-    </cacheField>
-    <cacheField name="Enjoyment" numFmtId="0">
-      <sharedItems containsMixedTypes="1" containsNumber="1" minValue="3.6666666666666665" maxValue="7"/>
+    <cacheField name="Learning Time (seconds)" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="68" maxValue="293"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -4691,66 +4715,414 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="12">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="24">
   <r>
     <n v="1"/>
     <x v="0"/>
-    <n v="192"/>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5.333333333333333"/>
+    <n v="5.333333333333333"/>
+    <n v="5.333333333333333"/>
+  </r>
+  <r>
+    <n v="1"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="3.6666666666666665"/>
+    <n v="4.333333333333333"/>
+    <n v="4.333333333333333"/>
   </r>
   <r>
     <n v="2"/>
     <x v="0"/>
-    <n v="293"/>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="7"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="6.333333333333333"/>
+    <n v="5.333333333333333"/>
+    <n v="7"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="5.333333333333333"/>
+    <n v="5"/>
+    <n v="6.666666666666667"/>
   </r>
   <r>
     <n v="3"/>
     <x v="0"/>
-    <n v="272"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="4.333333333333333"/>
+    <n v="5.333333333333333"/>
+    <n v="6.333333333333333"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="7"/>
+    <n v="6"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="4.333333333333333"/>
+    <n v="5.666666666666667"/>
+    <n v="6.333333333333333"/>
   </r>
   <r>
     <n v="4"/>
     <x v="0"/>
-    <n v="173"/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4.333333333333333"/>
+    <n v="4.666666666666667"/>
+    <n v="4"/>
   </r>
   <r>
-    <n v="5"/>
+    <n v="4"/>
+    <x v="0"/>
     <x v="1"/>
-    <n v="187"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="4.333333333333333"/>
+    <n v="5.333333333333333"/>
+    <n v="3.6666666666666665"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5.333333333333333"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="3"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3.3333333333333335"/>
+    <n v="3.3333333333333335"/>
+    <n v="4.666666666666667"/>
   </r>
   <r>
     <n v="6"/>
     <x v="1"/>
-    <n v="146"/>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="4.666666666666667"/>
+    <n v="5.666666666666667"/>
+    <n v="5.666666666666667"/>
+  </r>
+  <r>
+    <n v="6"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="2"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="3.6666666666666665"/>
+    <n v="4.333333333333333"/>
+    <n v="5.666666666666667"/>
   </r>
   <r>
     <n v="7"/>
     <x v="1"/>
-    <n v="242"/>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="3"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="5.666666666666667"/>
+    <n v="5.666666666666667"/>
+    <n v="5.666666666666667"/>
+  </r>
+  <r>
+    <n v="7"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="4.333333333333333"/>
+    <n v="5.333333333333333"/>
+    <n v="5"/>
   </r>
   <r>
     <n v="8"/>
     <x v="1"/>
-    <n v="134"/>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5.333333333333333"/>
+    <n v="4.333333333333333"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="8"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="2"/>
+    <n v="3"/>
+    <n v="2"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="5"/>
+    <n v="3.3333333333333335"/>
+    <n v="2.6666666666666665"/>
+    <n v="4.666666666666667"/>
   </r>
   <r>
     <n v="9"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5.333333333333333"/>
+    <n v="5"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="9"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
   </r>
   <r>
     <n v="10"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="4.666666666666667"/>
+    <n v="4.333333333333333"/>
+    <n v="5.333333333333333"/>
+  </r>
+  <r>
+    <n v="10"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="4.333333333333333"/>
+    <n v="5.666666666666667"/>
   </r>
   <r>
     <n v="11"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="3"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="4.333333333333333"/>
+    <n v="5.666666666666667"/>
+    <n v="5.666666666666667"/>
+  </r>
+  <r>
+    <n v="11"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="7"/>
+    <n v="5"/>
+    <n v="5.333333333333333"/>
+    <n v="6"/>
+    <n v="5"/>
   </r>
   <r>
     <n v="12"/>
     <x v="2"/>
-    <m/>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="6"/>
+    <n v="7"/>
+    <n v="7"/>
+    <n v="6.333333333333333"/>
+    <n v="6.333333333333333"/>
+    <n v="6.333333333333333"/>
+  </r>
+  <r>
+    <n v="12"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="6"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="4"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="6"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="5"/>
+    <n v="4.666666666666667"/>
   </r>
 </pivotCacheRecords>
 </file>
@@ -4889,484 +5261,136 @@
     <n v="9"/>
     <x v="2"/>
     <x v="0"/>
-    <m/>
-    <m/>
-    <n v="1"/>
+    <n v="54"/>
+    <n v="0"/>
+    <n v="0.82000000000000006"/>
   </r>
   <r>
     <n v="9"/>
     <x v="2"/>
     <x v="1"/>
-    <m/>
-    <m/>
-    <n v="1"/>
+    <n v="77"/>
+    <n v="0"/>
+    <n v="0.7433333333333334"/>
   </r>
   <r>
     <n v="10"/>
     <x v="2"/>
     <x v="0"/>
-    <m/>
-    <m/>
-    <n v="1"/>
+    <n v="27"/>
+    <n v="0"/>
+    <n v="0.91"/>
   </r>
   <r>
     <n v="10"/>
     <x v="2"/>
     <x v="1"/>
-    <m/>
-    <m/>
-    <n v="1"/>
+    <n v="45"/>
+    <n v="0"/>
+    <n v="0.85"/>
   </r>
   <r>
     <n v="11"/>
     <x v="2"/>
     <x v="0"/>
-    <m/>
-    <m/>
-    <n v="1"/>
+    <n v="40"/>
+    <n v="0"/>
+    <n v="0.8666666666666667"/>
   </r>
   <r>
     <n v="11"/>
     <x v="2"/>
     <x v="1"/>
-    <m/>
-    <m/>
-    <n v="1"/>
+    <n v="57"/>
+    <n v="0"/>
+    <n v="0.81"/>
   </r>
   <r>
     <n v="12"/>
     <x v="2"/>
     <x v="0"/>
-    <m/>
-    <m/>
-    <n v="1"/>
+    <n v="56"/>
+    <n v="0"/>
+    <n v="0.81333333333333335"/>
   </r>
   <r>
     <n v="12"/>
     <x v="2"/>
     <x v="1"/>
-    <m/>
-    <m/>
+    <n v="126"/>
     <n v="1"/>
+    <n v="0.58000000000000007"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="24">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="12">
   <r>
     <n v="1"/>
     <x v="0"/>
-    <x v="0"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5.333333333333333"/>
-    <n v="5.333333333333333"/>
-    <n v="5.333333333333333"/>
-  </r>
-  <r>
-    <n v="1"/>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="4"/>
-    <n v="2"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="3.6666666666666665"/>
-    <n v="4.333333333333333"/>
-    <n v="4.333333333333333"/>
+    <n v="192"/>
   </r>
   <r>
     <n v="2"/>
     <x v="0"/>
-    <x v="0"/>
-    <n v="6"/>
-    <n v="7"/>
-    <n v="7"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="7"/>
-    <n v="5"/>
-    <n v="7"/>
-    <n v="6.333333333333333"/>
-    <n v="5.333333333333333"/>
-    <n v="7"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="7"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="7"/>
-    <n v="5.333333333333333"/>
-    <n v="5"/>
-    <n v="6.666666666666667"/>
+    <n v="293"/>
   </r>
   <r>
     <n v="3"/>
     <x v="0"/>
-    <x v="0"/>
-    <n v="4"/>
-    <n v="5"/>
-    <n v="7"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="7"/>
-    <n v="4.333333333333333"/>
-    <n v="5.333333333333333"/>
-    <n v="6.333333333333333"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <x v="0"/>
-    <x v="1"/>
-    <n v="5"/>
-    <n v="7"/>
-    <n v="7"/>
-    <n v="6"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="7"/>
-    <n v="4.333333333333333"/>
-    <n v="5.666666666666667"/>
-    <n v="6.333333333333333"/>
+    <n v="272"/>
   </r>
   <r>
     <n v="4"/>
     <x v="0"/>
-    <x v="0"/>
-    <n v="4"/>
-    <n v="5"/>
-    <n v="4"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="3"/>
-    <n v="4"/>
-    <n v="5"/>
-    <n v="4"/>
-    <n v="4.333333333333333"/>
-    <n v="4.666666666666667"/>
-    <n v="4"/>
+    <n v="173"/>
   </r>
   <r>
-    <n v="4"/>
-    <x v="0"/>
+    <n v="5"/>
     <x v="1"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="4"/>
-    <n v="5"/>
-    <n v="4"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="6"/>
-    <n v="4"/>
-    <n v="4.333333333333333"/>
-    <n v="5.333333333333333"/>
-    <n v="3.6666666666666665"/>
-  </r>
-  <r>
-    <n v="5"/>
-    <x v="1"/>
-    <x v="0"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="4"/>
-    <n v="5"/>
-    <n v="4"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5.333333333333333"/>
-    <n v="5"/>
-  </r>
-  <r>
-    <n v="5"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="3"/>
-    <n v="4"/>
-    <n v="5"/>
-    <n v="4"/>
-    <n v="3"/>
-    <n v="3"/>
-    <n v="4"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="3.3333333333333335"/>
-    <n v="3.3333333333333335"/>
-    <n v="4.666666666666667"/>
+    <n v="187"/>
   </r>
   <r>
     <n v="6"/>
     <x v="1"/>
-    <x v="0"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="4.666666666666667"/>
-    <n v="5.666666666666667"/>
-    <n v="5.666666666666667"/>
-  </r>
-  <r>
-    <n v="6"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="2"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="3"/>
-    <n v="2"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="3.6666666666666665"/>
-    <n v="4.333333333333333"/>
-    <n v="5.666666666666667"/>
+    <n v="146"/>
   </r>
   <r>
     <n v="7"/>
     <x v="1"/>
-    <x v="0"/>
-    <n v="6"/>
-    <n v="7"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="7"/>
-    <n v="3"/>
-    <n v="6"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="5.666666666666667"/>
-    <n v="5.666666666666667"/>
-    <n v="5.666666666666667"/>
-  </r>
-  <r>
-    <n v="7"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="4"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="4"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="4.333333333333333"/>
-    <n v="5.333333333333333"/>
-    <n v="5"/>
+    <n v="242"/>
   </r>
   <r>
     <n v="8"/>
     <x v="1"/>
-    <x v="0"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="2"/>
-    <n v="5"/>
-    <n v="6"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="5.333333333333333"/>
-    <n v="4.333333333333333"/>
-    <n v="5"/>
-  </r>
-  <r>
-    <n v="8"/>
-    <x v="1"/>
-    <x v="1"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="5"/>
-    <n v="2"/>
-    <n v="3"/>
-    <n v="2"/>
-    <n v="4"/>
-    <n v="3"/>
-    <n v="5"/>
-    <n v="3.3333333333333335"/>
-    <n v="2.6666666666666665"/>
-    <n v="4.666666666666667"/>
+    <n v="134"/>
   </r>
   <r>
     <n v="9"/>
     <x v="2"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-  </r>
-  <r>
-    <n v="9"/>
-    <x v="2"/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
+    <n v="68"/>
   </r>
   <r>
     <n v="10"/>
     <x v="2"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-  </r>
-  <r>
-    <n v="10"/>
-    <x v="2"/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
+    <n v="172"/>
   </r>
   <r>
     <n v="11"/>
     <x v="2"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-  </r>
-  <r>
-    <n v="11"/>
-    <x v="2"/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
+    <n v="166"/>
   </r>
   <r>
     <n v="12"/>
     <x v="2"/>
-    <x v="0"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-  </r>
-  <r>
-    <n v="12"/>
-    <x v="2"/>
-    <x v="1"/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <m/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
-    <e v="#DIV/0!"/>
+    <n v="133"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="obj_time" cacheId="67" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Control x Task">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="obj_time" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Control x Task">
   <location ref="A62:B74" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5458,7 +5482,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="obj_errors" cacheId="67" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Control x Task">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="obj_errors" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Control x Task">
   <location ref="A47:B59" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5550,7 +5574,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="learning" cacheId="63" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Control ">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="learning" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Control ">
   <location ref="A77:B81" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField showAll="0"/>
@@ -5597,7 +5621,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="objective" cacheId="67" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Control x Task">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="objective" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Control x Task">
   <location ref="A32:B44" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5689,7 +5713,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="subjective" cacheId="71" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Control x Task">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="subjective" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Control x Task">
   <location ref="A2:J14" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5816,7 +5840,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="71" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Control x Task">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2" rowHeaderCaption="Control x Task">
   <location ref="A17:D29" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="15">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -5956,9 +5980,7 @@
     <tableColumn id="3" name="Task Type"/>
     <tableColumn id="5" name="Task Time (seconds)"/>
     <tableColumn id="7" name="Errors"/>
-    <tableColumn id="6" name="Score (max time = 5 min)" dataDxfId="11">
-      <calculatedColumnFormula>1-obj[[#This Row],[Task Time (seconds)]]/300</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="6" name="Score (max time = 5 min)" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5992,15 +6014,9 @@
     <tableColumn id="10" name="satisfied"/>
     <tableColumn id="11" name="useful"/>
     <tableColumn id="12" name="happy"/>
-    <tableColumn id="13" name="Ease of Use" dataDxfId="2">
-      <calculatedColumnFormula>AVERAGE(E4,H4,I4)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="14" name="Usefulness" dataDxfId="1">
-      <calculatedColumnFormula>AVERAGE(D4,G4,K4)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="15" name="Enjoyment" dataDxfId="0">
-      <calculatedColumnFormula>AVERAGE(F4,J4,L4)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="13" name="Ease of Use" dataDxfId="2"/>
+    <tableColumn id="14" name="Usefulness" dataDxfId="1"/>
+    <tableColumn id="15" name="Enjoyment" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6287,7 +6303,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6338,7 +6354,6 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.8833333333333333</v>
       </c>
     </row>
@@ -6359,7 +6374,6 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.88</v>
       </c>
     </row>
@@ -6380,7 +6394,6 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.89666666666666672</v>
       </c>
     </row>
@@ -6401,7 +6414,6 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.87333333333333329</v>
       </c>
     </row>
@@ -6422,7 +6434,6 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.89666666666666672</v>
       </c>
     </row>
@@ -6443,7 +6454,6 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.73333333333333339</v>
       </c>
     </row>
@@ -6464,7 +6474,6 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.82666666666666666</v>
       </c>
     </row>
@@ -6485,7 +6494,6 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.78333333333333333</v>
       </c>
     </row>
@@ -6506,7 +6514,6 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.89666666666666672</v>
       </c>
     </row>
@@ -6527,7 +6534,6 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.41000000000000003</v>
       </c>
     </row>
@@ -6548,7 +6554,6 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.90666666666666662</v>
       </c>
     </row>
@@ -6569,7 +6574,6 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.68666666666666665</v>
       </c>
     </row>
@@ -6590,7 +6594,6 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.84</v>
       </c>
     </row>
@@ -6611,7 +6614,6 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.64333333333333331</v>
       </c>
     </row>
@@ -6632,7 +6634,6 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.92999999999999994</v>
       </c>
     </row>
@@ -6653,7 +6654,6 @@
         <v>3</v>
       </c>
       <c r="F17">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
         <v>0.47333333333333338</v>
       </c>
     </row>
@@ -6667,9 +6667,14 @@
       <c r="C18" t="s">
         <v>11</v>
       </c>
+      <c r="D18">
+        <v>54</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
       <c r="F18">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.82000000000000006</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -6682,9 +6687,14 @@
       <c r="C19" t="s">
         <v>12</v>
       </c>
+      <c r="D19">
+        <v>77</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
       <c r="F19">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.7433333333333334</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -6697,9 +6707,14 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
+      <c r="D20">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
       <c r="F20">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -6712,9 +6727,14 @@
       <c r="C21" t="s">
         <v>12</v>
       </c>
+      <c r="D21">
+        <v>45</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
       <c r="F21">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -6727,9 +6747,14 @@
       <c r="C22" t="s">
         <v>11</v>
       </c>
+      <c r="D22">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
       <c r="F22">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -6742,9 +6767,14 @@
       <c r="C23" t="s">
         <v>12</v>
       </c>
+      <c r="D23">
+        <v>57</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
       <c r="F23">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -6757,9 +6787,14 @@
       <c r="C24" t="s">
         <v>11</v>
       </c>
+      <c r="D24">
+        <v>56</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
       <c r="F24">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.81333333333333335</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -6772,9 +6807,14 @@
       <c r="C25" t="s">
         <v>12</v>
       </c>
+      <c r="D25">
+        <v>126</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
       <c r="F25">
-        <f>1-obj[[#This Row],[Task Time (seconds)]]/300</f>
-        <v>1</v>
+        <v>0.58000000000000007</v>
       </c>
     </row>
   </sheetData>
@@ -6790,7 +6830,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6907,7 +6947,9 @@
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4">
+        <v>68</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -6916,7 +6958,9 @@
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4">
+        <v>172</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
@@ -6925,7 +6969,9 @@
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4">
+        <v>166</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
@@ -6934,7 +6980,9 @@
       <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4">
+        <v>133</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6949,8 +6997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7117,15 +7165,12 @@
         <v>5</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M27" si="0">AVERAGE(E4,H4,I4)</f>
         <v>5.333333333333333</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N27" si="1">AVERAGE(D4,G4,K4)</f>
         <v>5.333333333333333</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O27" si="2">AVERAGE(F4,J4,L4)</f>
         <v>5.333333333333333</v>
       </c>
     </row>
@@ -7167,15 +7212,12 @@
         <v>5</v>
       </c>
       <c r="M5">
-        <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="N5">
-        <f t="shared" si="1"/>
         <v>4.333333333333333</v>
       </c>
       <c r="O5">
-        <f t="shared" si="2"/>
         <v>4.333333333333333</v>
       </c>
     </row>
@@ -7217,15 +7259,12 @@
         <v>7</v>
       </c>
       <c r="M6">
-        <f t="shared" si="0"/>
         <v>6.333333333333333</v>
       </c>
       <c r="N6">
-        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
       <c r="O6">
-        <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
@@ -7267,15 +7306,12 @@
         <v>7</v>
       </c>
       <c r="M7">
-        <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
       <c r="N7">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="O7">
-        <f t="shared" si="2"/>
         <v>6.666666666666667</v>
       </c>
     </row>
@@ -7317,15 +7353,12 @@
         <v>7</v>
       </c>
       <c r="M8">
-        <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
       <c r="N8">
-        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
       <c r="O8">
-        <f t="shared" si="2"/>
         <v>6.333333333333333</v>
       </c>
     </row>
@@ -7367,15 +7400,12 @@
         <v>7</v>
       </c>
       <c r="M9">
-        <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
       <c r="N9">
-        <f t="shared" si="1"/>
         <v>5.666666666666667</v>
       </c>
       <c r="O9">
-        <f t="shared" si="2"/>
         <v>6.333333333333333</v>
       </c>
     </row>
@@ -7417,15 +7447,12 @@
         <v>4</v>
       </c>
       <c r="M10">
-        <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
       <c r="N10">
-        <f t="shared" si="1"/>
         <v>4.666666666666667</v>
       </c>
       <c r="O10">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
@@ -7467,15 +7494,12 @@
         <v>4</v>
       </c>
       <c r="M11">
-        <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
       <c r="N11">
-        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
       <c r="O11">
-        <f t="shared" si="2"/>
         <v>3.6666666666666665</v>
       </c>
     </row>
@@ -7517,15 +7541,12 @@
         <v>5</v>
       </c>
       <c r="M12">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="N12">
-        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
       <c r="O12">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
@@ -7567,15 +7588,12 @@
         <v>5</v>
       </c>
       <c r="M13">
-        <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="N13">
-        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="O13">
-        <f t="shared" si="2"/>
         <v>4.666666666666667</v>
       </c>
     </row>
@@ -7617,15 +7635,12 @@
         <v>6</v>
       </c>
       <c r="M14">
-        <f t="shared" si="0"/>
         <v>4.666666666666667</v>
       </c>
       <c r="N14">
-        <f t="shared" si="1"/>
         <v>5.666666666666667</v>
       </c>
       <c r="O14">
-        <f t="shared" si="2"/>
         <v>5.666666666666667</v>
       </c>
     </row>
@@ -7667,15 +7682,12 @@
         <v>6</v>
       </c>
       <c r="M15">
-        <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="N15">
-        <f t="shared" si="1"/>
         <v>4.333333333333333</v>
       </c>
       <c r="O15">
-        <f t="shared" si="2"/>
         <v>5.666666666666667</v>
       </c>
     </row>
@@ -7717,15 +7729,12 @@
         <v>5</v>
       </c>
       <c r="M16">
-        <f t="shared" si="0"/>
         <v>5.666666666666667</v>
       </c>
       <c r="N16">
-        <f t="shared" si="1"/>
         <v>5.666666666666667</v>
       </c>
       <c r="O16">
-        <f t="shared" si="2"/>
         <v>5.666666666666667</v>
       </c>
     </row>
@@ -7767,15 +7776,12 @@
         <v>5</v>
       </c>
       <c r="M17">
-        <f t="shared" si="0"/>
         <v>4.333333333333333</v>
       </c>
       <c r="N17">
-        <f t="shared" si="1"/>
         <v>5.333333333333333</v>
       </c>
       <c r="O17">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
@@ -7817,15 +7823,12 @@
         <v>5</v>
       </c>
       <c r="M18">
-        <f t="shared" si="0"/>
         <v>5.333333333333333</v>
       </c>
       <c r="N18">
-        <f t="shared" si="1"/>
         <v>4.333333333333333</v>
       </c>
       <c r="O18">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
     </row>
@@ -7867,15 +7870,12 @@
         <v>5</v>
       </c>
       <c r="M19">
-        <f t="shared" si="0"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="N19">
-        <f t="shared" si="1"/>
         <v>2.6666666666666665</v>
       </c>
       <c r="O19">
-        <f t="shared" si="2"/>
         <v>4.666666666666667</v>
       </c>
     </row>
@@ -7889,17 +7889,41 @@
       <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="M20" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N20" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O20" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>6</v>
+      </c>
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>6</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20">
+        <v>5</v>
+      </c>
+      <c r="M20">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="N20">
+        <v>5</v>
+      </c>
+      <c r="O20">
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
@@ -7912,17 +7936,41 @@
       <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="M21" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N21" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O21" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>6</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <v>5</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>5</v>
+      </c>
+      <c r="O21">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
@@ -7935,17 +7983,41 @@
       <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="M22" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N22" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O22" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="I22">
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>6</v>
+      </c>
+      <c r="M22">
+        <v>4.666666666666667</v>
+      </c>
+      <c r="N22">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="O22">
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
@@ -7958,17 +8030,41 @@
       <c r="C23" t="s">
         <v>12</v>
       </c>
-      <c r="M23" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N23" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O23" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23">
+        <v>5</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23">
+        <v>6</v>
+      </c>
+      <c r="M23">
+        <v>4</v>
+      </c>
+      <c r="N23">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="O23">
+        <v>5.666666666666667</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
@@ -7981,17 +8077,41 @@
       <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="M24" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N24" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O24" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D24">
+        <v>5</v>
+      </c>
+      <c r="E24">
+        <v>6</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>6</v>
+      </c>
+      <c r="K24">
+        <v>6</v>
+      </c>
+      <c r="L24">
+        <v>5</v>
+      </c>
+      <c r="M24">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="N24">
+        <v>5.666666666666667</v>
+      </c>
+      <c r="O24">
+        <v>5.666666666666667</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
@@ -8004,17 +8124,41 @@
       <c r="C25" t="s">
         <v>12</v>
       </c>
-      <c r="M25" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N25" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O25" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25">
+        <v>6</v>
+      </c>
+      <c r="F25">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25">
+        <v>6</v>
+      </c>
+      <c r="I25">
+        <v>4</v>
+      </c>
+      <c r="J25">
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>7</v>
+      </c>
+      <c r="L25">
+        <v>5</v>
+      </c>
+      <c r="M25">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="N25">
+        <v>6</v>
+      </c>
+      <c r="O25">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -8027,17 +8171,41 @@
       <c r="C26" t="s">
         <v>11</v>
       </c>
-      <c r="M26" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N26" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O26" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26">
+        <v>6</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>7</v>
+      </c>
+      <c r="J26">
+        <v>6</v>
+      </c>
+      <c r="K26">
+        <v>7</v>
+      </c>
+      <c r="L26">
+        <v>7</v>
+      </c>
+      <c r="M26">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="N26">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="O26">
+        <v>6.333333333333333</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -8050,17 +8218,41 @@
       <c r="C27" t="s">
         <v>12</v>
       </c>
-      <c r="M27" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O27" t="e">
-        <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>6</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <v>5</v>
+      </c>
+      <c r="K27">
+        <v>6</v>
+      </c>
+      <c r="L27">
+        <v>5</v>
+      </c>
+      <c r="M27">
+        <v>5</v>
+      </c>
+      <c r="N27">
+        <v>5</v>
+      </c>
+      <c r="O27">
+        <v>4.666666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -8077,7 +8269,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8274,20 +8466,80 @@
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
+      </c>
+      <c r="B13">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -8308,8 +8560,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
@@ -8370,43 +8622,97 @@
       <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
+      <c r="B4" s="9">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="D4" s="9">
+        <v>5.75</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="F4" s="9">
+        <v>5.25</v>
+      </c>
+      <c r="G4" s="9">
+        <v>4.75</v>
+      </c>
+      <c r="H4" s="9">
+        <v>5.25</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="J4" s="9">
+        <v>5.75</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
+      <c r="B5" s="9">
+        <v>4.75</v>
+      </c>
+      <c r="C5" s="9">
+        <v>5.25</v>
+      </c>
+      <c r="D5" s="9">
+        <v>5.25</v>
+      </c>
+      <c r="E5" s="9">
+        <v>5</v>
+      </c>
+      <c r="F5" s="9">
+        <v>5</v>
+      </c>
+      <c r="G5" s="9">
+        <v>4.25</v>
+      </c>
+      <c r="H5" s="9">
+        <v>4.75</v>
+      </c>
+      <c r="I5" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="J5" s="9">
+        <v>5.25</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
+      <c r="B6" s="9">
+        <v>4.875</v>
+      </c>
+      <c r="C6" s="9">
+        <v>5.375</v>
+      </c>
+      <c r="D6" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="E6" s="9">
+        <v>5.25</v>
+      </c>
+      <c r="F6" s="9">
+        <v>5.125</v>
+      </c>
+      <c r="G6" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="H6" s="9">
+        <v>5</v>
+      </c>
+      <c r="I6" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="J6" s="9">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -8666,42 +8972,42 @@
       <c r="A19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="9" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C19" s="9" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D19" s="9" t="e">
-        <v>#DIV/0!</v>
+      <c r="B19" s="9">
+        <v>5.1666666666666661</v>
+      </c>
+      <c r="C19" s="9">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="D19" s="9">
+        <v>5.583333333333333</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="9" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C20" s="9" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D20" s="9" t="e">
-        <v>#DIV/0!</v>
+      <c r="B20" s="9">
+        <v>4.833333333333333</v>
+      </c>
+      <c r="C20" s="9">
+        <v>5.083333333333333</v>
+      </c>
+      <c r="D20" s="9">
+        <v>5.0833333333333339</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="9" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C21" s="9" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D21" s="9" t="e">
-        <v>#DIV/0!</v>
+      <c r="B21" s="9">
+        <v>5</v>
+      </c>
+      <c r="C21" s="9">
+        <v>5.208333333333333</v>
+      </c>
+      <c r="D21" s="9">
+        <v>5.333333333333333</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -8823,7 +9129,7 @@
         <v>11</v>
       </c>
       <c r="B34" s="9">
-        <v>1</v>
+        <v>0.85250000000000004</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -8831,7 +9137,7 @@
         <v>12</v>
       </c>
       <c r="B35" s="9">
-        <v>1</v>
+        <v>0.74583333333333335</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -8839,7 +9145,7 @@
         <v>57</v>
       </c>
       <c r="B36" s="9">
-        <v>1</v>
+        <v>0.79916666666666658</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -8920,19 +9226,25 @@
       <c r="A49" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B49" s="9"/>
+      <c r="B49" s="9">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B50" s="9"/>
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="9"/>
+      <c r="B51" s="9">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
@@ -9012,19 +9324,25 @@
       <c r="A64" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B64" s="9"/>
+      <c r="B64" s="9">
+        <v>44.25</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B65" s="9"/>
+      <c r="B65" s="9">
+        <v>76.25</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B66" s="9"/>
+      <c r="B66" s="9">
+        <v>60.25</v>
+      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
@@ -9098,7 +9416,9 @@
       <c r="A78" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B78" s="9"/>
+      <c r="B78" s="9">
+        <v>134.75</v>
+      </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
@@ -9121,7 +9441,7 @@
         <v>47</v>
       </c>
       <c r="B81" s="9">
-        <v>204.875</v>
+        <v>181.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>